<commit_message>
Add 'historical' to deleted values
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-deleteQuestions-2.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-deleteQuestions-2.xlsx
@@ -143,7 +143,7 @@
     <t xml:space="preserve">deletemetoo</t>
   </si>
   <si>
-    <t xml:space="preserve">hidden</t>
+    <t xml:space="preserve">historical</t>
   </si>
   <si>
     <t xml:space="preserve">dontdeleteme</t>
@@ -274,7 +274,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.89"/>
@@ -1370,11 +1370,11 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.56"/>

</xml_diff>

<commit_message>
EPI-573 Data deletion tasks survey screen components (#4721)
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-deleteQuestions-2.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-deleteQuestions-2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC7C4C-A04B-AB45-8415-1F29E2045700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAE9F00-AE54-F146-A6FE-74FBEA263ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25900" windowHeight="13160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>programName</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Post-deletion</t>
   </si>
   <si>
-    <t>deleted</t>
-  </si>
-  <si>
     <t>deletemetoo</t>
   </si>
   <si>
@@ -163,13 +160,16 @@
   </si>
   <si>
     <t>dontdeleteme</t>
+  </si>
+  <si>
+    <t>current</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -180,7 +180,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,9 +209,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1619,7 +1626,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1691,13 +1698,13 @@
       <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P2" t="s">
-        <v>38</v>
+      <c r="P2" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>36</v>
@@ -1705,19 +1712,22 @@
       <c r="D3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P3" t="s">
-        <v>40</v>
+      <c r="P3" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="P4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>